<commit_message>
Lesson 13 Change cells 02nd
</commit_message>
<xml_diff>
--- a/tutorial_02.xlsx
+++ b/tutorial_02.xlsx
@@ -1,43 +1,113 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="360" yWindow="45" windowWidth="11475" windowHeight="9795" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="11475" windowHeight="9795"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="145621" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Names</t>
+  </si>
+  <si>
+    <t>Favourite Colour</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>Soft Stone</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Magenta</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Luke</t>
+  </si>
+  <si>
+    <t>Jade</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Hazel</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Mathew</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Bartholomew</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -56,81 +126,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,188 +428,131 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Names</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Favourite Colour</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Brian</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Soft Stone</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Blue</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Paul</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Magenta</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Peter</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Green</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Luke</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Jade</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Hazel</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Thomas</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Red</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Mathew</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Pink</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Simon</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Judas</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Orange</t>
-        </is>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967292" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Lesson 14 Update via loop
</commit_message>
<xml_diff>
--- a/tutorial_02.xlsx
+++ b/tutorial_02.xlsx
@@ -1,113 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="11475" windowHeight="9795"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="360" yWindow="45" windowWidth="11475" windowHeight="9795" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Names</t>
-  </si>
-  <si>
-    <t>Favourite Colour</t>
-  </si>
-  <si>
-    <t>Brian</t>
-  </si>
-  <si>
-    <t>Soft Stone</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Paul</t>
-  </si>
-  <si>
-    <t>Magenta</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Luke</t>
-  </si>
-  <si>
-    <t>Jade</t>
-  </si>
-  <si>
-    <t>Andrew</t>
-  </si>
-  <si>
-    <t>Hazel</t>
-  </si>
-  <si>
-    <t>Thomas</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Mathew</t>
-  </si>
-  <si>
-    <t>Pink</t>
-  </si>
-  <si>
-    <t>Simon</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>Bartholomew</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -126,19 +56,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -428,131 +420,212 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col width="13.140625" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
+    <row r="1" customFormat="1" s="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Favourite Colour</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Soft Stone</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Magenta</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Peter</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Luke</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Jade</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Andrew</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Hazel</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Thomas</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Mathew</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Bartholomew</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967292" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>